<commit_message>
Import Export Items change
</commit_message>
<xml_diff>
--- a/client/src/assets/sample/ctordering_items.xlsx
+++ b/client/src/assets/sample/ctordering_items.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krunal/Project/Finished/foodup/client/src/assets/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -32,13 +35,13 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Order No</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
-    <t>Category Name</t>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Order</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,13 +434,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import Item image added
</commit_message>
<xml_diff>
--- a/client/src/assets/sample/ctordering_items.xlsx
+++ b/client/src/assets/sample/ctordering_items.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krunal/Project/Finished/foodup/client/src/assets/sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krunal/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,7 +429,7 @@
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,6 +444,9 @@
       </c>
       <c r="E1" t="s">
         <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add special price field
</commit_message>
<xml_diff>
--- a/client/src/assets/sample/ctordering_items.xlsx
+++ b/client/src/assets/sample/ctordering_items.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krunal/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Softices/personal/workspace/ruby/foodup-github/client/src/assets/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,9 +16,6 @@
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -45,6 +42,9 @@
   </si>
   <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>SpecialPrice</t>
   </si>
 </sst>
 </file>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,7 +429,7 @@
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,15 +437,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>